<commit_message>
db: create first full vershion db
</commit_message>
<xml_diff>
--- a/database/data_for_import/data_for_import.xlsx
+++ b/database/data_for_import/data_for_import.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Progects\study_1c\database\data_for_import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Progect\pp+diplom\study_1c\database\data_for_import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9692BE75-FA95-4F45-82F4-DA7D948C1D90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C14D30-C578-45D2-B8A8-E975FFD57B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="775" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" tabRatio="775" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="roles" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="306">
   <si>
     <t>role_id</t>
   </si>
@@ -482,21 +482,9 @@
     <t>task_number_of_block</t>
   </si>
   <si>
-    <t>27c7f513-82d2-49ea-a494-b797bb15d7f6</t>
-  </si>
-  <si>
-    <t>27c7f513-82d2-49ea-a494-b797bb15d7f7</t>
-  </si>
-  <si>
-    <t>27c7f513-82d2-49ea-a494-b797bb15d7f8</t>
-  </si>
-  <si>
     <t>Объекты справочной информации</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Документооборот торгового предприятия</t>
   </si>
   <si>
@@ -557,72 +545,6 @@
     <t>Начало работы с платформой «1С:Предприятие 8» (Бухгалтерию качать не нужно и 8.2 версию тоже) Только качать платформу 8.3</t>
   </si>
   <si>
-    <t>27c7f513-82d2-49ea-a494-b797bb15d7f9</t>
-  </si>
-  <si>
-    <t>27c7f513-82d2-49ea-a494-b797bb15d7f10</t>
-  </si>
-  <si>
-    <t>27c7f513-82d2-49ea-a494-b797bb15d7f11</t>
-  </si>
-  <si>
-    <t>27c7f513-82d2-49ea-a494-b797bb15d7f12</t>
-  </si>
-  <si>
-    <t>27c7f513-82d2-49ea-a494-b797bb15d7f13</t>
-  </si>
-  <si>
-    <t>27c7f513-82d2-49ea-a494-b797bb15d7f14</t>
-  </si>
-  <si>
-    <t>27c7f513-82d2-49ea-a494-b797bb15d7f15</t>
-  </si>
-  <si>
-    <t>27c7f513-82d2-49ea-a494-b797bb15d7f16</t>
-  </si>
-  <si>
-    <t>27c7f513-82d2-49ea-a494-b797bb15d7f17</t>
-  </si>
-  <si>
-    <t>27c7f513-82d2-49ea-a494-b797bb15d7f18</t>
-  </si>
-  <si>
-    <t>27c7f513-82d2-49ea-a494-b797bb15d7f19</t>
-  </si>
-  <si>
-    <t>27c7f513-82d2-49ea-a494-b797bb15d7f20</t>
-  </si>
-  <si>
-    <t>27c7f513-82d2-49ea-a494-b797bb15d7f21</t>
-  </si>
-  <si>
-    <t>27c7f513-82d2-49ea-a494-b797bb15d7f22</t>
-  </si>
-  <si>
-    <t>27c7f513-82d2-49ea-a494-b797bb15d7f23</t>
-  </si>
-  <si>
-    <t>27c7f513-82d2-49ea-a494-b797bb15d7f24</t>
-  </si>
-  <si>
-    <t>27c7f513-82d2-49ea-a494-b797bb15d7f25</t>
-  </si>
-  <si>
-    <t>da772850-eae8-4538-a31e-81a550bfae63</t>
-  </si>
-  <si>
-    <t>da772850-eae8-4538-a31e-81a550bfae64</t>
-  </si>
-  <si>
-    <t>da772850-eae8-4538-a31e-81a550bfae65</t>
-  </si>
-  <si>
-    <t>da772850-eae8-4538-a31e-81a550bfae66</t>
-  </si>
-  <si>
-    <t>da772850-eae8-4538-a31e-81a550bfae67</t>
-  </si>
-  <si>
     <t>Изучаем язык 1С</t>
   </si>
   <si>
@@ -720,81 +642,6 @@
   </si>
   <si>
     <t>Задание 25</t>
-  </si>
-  <si>
-    <t>2acc63f9-a297-4f90-a0b8-2ffddbdfb3f3</t>
-  </si>
-  <si>
-    <t>2acc63f9-a297-4f90-a0b8-2ffddbdfb3f4</t>
-  </si>
-  <si>
-    <t>2acc63f9-a297-4f90-a0b8-2ffddbdfb3f5</t>
-  </si>
-  <si>
-    <t>2acc63f9-a297-4f90-a0b8-2ffddbdfb3f6</t>
-  </si>
-  <si>
-    <t>2acc63f9-a297-4f90-a0b8-2ffddbdfb3f7</t>
-  </si>
-  <si>
-    <t>2acc63f9-a297-4f90-a0b8-2ffddbdfb3f8</t>
-  </si>
-  <si>
-    <t>2acc63f9-a297-4f90-a0b8-2ffddbdfb3f9</t>
-  </si>
-  <si>
-    <t>2acc63f9-a297-4f90-a0b8-2ffddbdfb3f10</t>
-  </si>
-  <si>
-    <t>2acc63f9-a297-4f90-a0b8-2ffddbdfb3f11</t>
-  </si>
-  <si>
-    <t>2acc63f9-a297-4f90-a0b8-2ffddbdfb3f12</t>
-  </si>
-  <si>
-    <t>2acc63f9-a297-4f90-a0b8-2ffddbdfb3f13</t>
-  </si>
-  <si>
-    <t>2acc63f9-a297-4f90-a0b8-2ffddbdfb3f14</t>
-  </si>
-  <si>
-    <t>2acc63f9-a297-4f90-a0b8-2ffddbdfb3f15</t>
-  </si>
-  <si>
-    <t>2acc63f9-a297-4f90-a0b8-2ffddbdfb3f16</t>
-  </si>
-  <si>
-    <t>2acc63f9-a297-4f90-a0b8-2ffddbdfb3f17</t>
-  </si>
-  <si>
-    <t>2acc63f9-a297-4f90-a0b8-2ffddbdfb3f18</t>
-  </si>
-  <si>
-    <t>2acc63f9-a297-4f90-a0b8-2ffddbdfb3f19</t>
-  </si>
-  <si>
-    <t>2acc63f9-a297-4f90-a0b8-2ffddbdfb3f20</t>
-  </si>
-  <si>
-    <t>2acc63f9-a297-4f90-a0b8-2ffddbdfb3f21</t>
-  </si>
-  <si>
-    <t>2acc63f9-a297-4f90-a0b8-2ffddbdfb3f22</t>
-  </si>
-  <si>
-    <t>2acc63f9-a297-4f90-a0b8-2ffddbdfb3f23</t>
-  </si>
-  <si>
-    <t>2acc63f9-a297-4f90-a0b8-2ffddbdfb3f24</t>
-  </si>
-  <si>
-    <t>2acc63f9-a297-4f90-a0b8-2ffddbdfb3f25</t>
-  </si>
-  <si>
-    <t>2acc63f9-a297-4f90-a0b8-2ffddbdfb3f26</t>
-  </si>
-  <si>
-    <t>2acc63f9-a297-4f90-a0b8-2ffddbdfb3f27</t>
   </si>
   <si>
     <t>93448e94-18e5-4b12-b605-cbc386645125</t>
@@ -1162,7 +1009,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -1245,8 +1092,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -1531,10 +1378,13 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -1568,18 +1418,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4884ACB8-CF81-4DD8-BC47-C124E0924889}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:A38"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1602,475 +1453,553 @@
         <v>63</v>
       </c>
       <c r="G1" t="s">
-        <v>356</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>330</v>
+        <v>279</v>
       </c>
       <c r="B2" t="s">
-        <v>186</v>
+        <v>160</v>
       </c>
       <c r="C2" s="5">
         <f t="shared" ref="C2:C27" ca="1" si="0">NOW()</f>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D2">
         <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>264</v>
+        <v>213</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>331</v>
+        <v>280</v>
       </c>
       <c r="B3" t="s">
-        <v>187</v>
+        <v>161</v>
       </c>
       <c r="C3" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D3">
         <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>265</v>
+        <v>214</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>332</v>
+        <v>281</v>
       </c>
       <c r="B4" t="s">
-        <v>188</v>
+        <v>162</v>
       </c>
       <c r="C4" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D4">
         <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>266</v>
+        <v>215</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>333</v>
+        <v>282</v>
       </c>
       <c r="B5" t="s">
-        <v>189</v>
+        <v>163</v>
       </c>
       <c r="C5" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D5">
         <v>120</v>
       </c>
       <c r="F5" t="s">
-        <v>267</v>
+        <v>216</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>334</v>
+        <v>283</v>
       </c>
       <c r="B6" t="s">
-        <v>190</v>
+        <v>164</v>
       </c>
       <c r="C6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D6">
         <v>60</v>
       </c>
       <c r="F6" t="s">
-        <v>268</v>
+        <v>217</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>335</v>
+        <v>284</v>
       </c>
       <c r="B7" t="s">
-        <v>191</v>
+        <v>165</v>
       </c>
       <c r="C7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D7">
         <v>5</v>
       </c>
       <c r="F7" t="s">
-        <v>269</v>
+        <v>218</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>336</v>
+        <v>285</v>
       </c>
       <c r="B8" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
       <c r="C8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D8">
         <v>25</v>
       </c>
       <c r="F8" t="s">
-        <v>270</v>
+        <v>219</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>337</v>
+        <v>286</v>
       </c>
       <c r="B9" t="s">
-        <v>193</v>
+        <v>167</v>
       </c>
       <c r="C9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D9">
         <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>271</v>
+        <v>220</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>338</v>
+        <v>287</v>
       </c>
       <c r="B10" t="s">
-        <v>194</v>
+        <v>168</v>
       </c>
       <c r="C10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D10">
         <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>272</v>
+        <v>221</v>
+      </c>
+      <c r="G10">
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>339</v>
+        <v>288</v>
       </c>
       <c r="B11" t="s">
-        <v>195</v>
+        <v>169</v>
       </c>
       <c r="C11" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D11">
         <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>273</v>
+        <v>222</v>
+      </c>
+      <c r="G11">
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>340</v>
+        <v>289</v>
       </c>
       <c r="B12" t="s">
-        <v>196</v>
+        <v>170</v>
       </c>
       <c r="C12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D12">
         <v>25</v>
       </c>
       <c r="F12" t="s">
-        <v>274</v>
+        <v>223</v>
+      </c>
+      <c r="G12">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>341</v>
+        <v>290</v>
       </c>
       <c r="B13" t="s">
-        <v>197</v>
+        <v>171</v>
       </c>
       <c r="C13" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D13">
         <v>40</v>
       </c>
       <c r="F13" t="s">
-        <v>275</v>
+        <v>224</v>
+      </c>
+      <c r="G13">
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>342</v>
+        <v>291</v>
       </c>
       <c r="B14" t="s">
-        <v>198</v>
+        <v>172</v>
       </c>
       <c r="C14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D14">
         <v>25</v>
       </c>
       <c r="F14" t="s">
-        <v>276</v>
+        <v>225</v>
+      </c>
+      <c r="G14">
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>343</v>
+        <v>292</v>
       </c>
       <c r="B15" t="s">
-        <v>199</v>
+        <v>173</v>
       </c>
       <c r="C15" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D15">
         <v>90</v>
       </c>
       <c r="F15" t="s">
-        <v>277</v>
+        <v>226</v>
+      </c>
+      <c r="G15">
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>344</v>
+        <v>293</v>
       </c>
       <c r="B16" t="s">
-        <v>200</v>
+        <v>174</v>
       </c>
       <c r="C16" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D16">
         <v>90</v>
       </c>
       <c r="F16" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>227</v>
+      </c>
+      <c r="G16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>345</v>
+        <v>294</v>
       </c>
       <c r="B17" t="s">
-        <v>201</v>
+        <v>175</v>
       </c>
       <c r="C17" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D17">
         <v>5</v>
       </c>
       <c r="F17" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>228</v>
+      </c>
+      <c r="G17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>346</v>
+        <v>295</v>
       </c>
       <c r="B18" t="s">
-        <v>202</v>
+        <v>176</v>
       </c>
       <c r="C18" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D18">
         <v>5</v>
       </c>
       <c r="F18" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>229</v>
+      </c>
+      <c r="G18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>347</v>
+        <v>296</v>
       </c>
       <c r="B19" t="s">
-        <v>203</v>
+        <v>177</v>
       </c>
       <c r="C19" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D19">
         <v>90</v>
       </c>
       <c r="F19" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>230</v>
+      </c>
+      <c r="G19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>348</v>
+        <v>297</v>
       </c>
       <c r="B20" t="s">
-        <v>204</v>
+        <v>178</v>
       </c>
       <c r="C20" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D20">
         <v>25</v>
       </c>
       <c r="F20" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>231</v>
+      </c>
+      <c r="G20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>349</v>
+        <v>298</v>
       </c>
       <c r="B21" t="s">
-        <v>205</v>
+        <v>179</v>
       </c>
       <c r="C21" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D21">
         <v>120</v>
       </c>
       <c r="F21" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>232</v>
+      </c>
+      <c r="G21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>350</v>
+        <v>299</v>
       </c>
       <c r="B22" t="s">
-        <v>206</v>
+        <v>180</v>
       </c>
       <c r="C22" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D22">
         <v>50</v>
       </c>
       <c r="F22" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>233</v>
+      </c>
+      <c r="G22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>351</v>
+        <v>300</v>
       </c>
       <c r="B23" t="s">
-        <v>207</v>
+        <v>181</v>
       </c>
       <c r="C23" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D23">
         <v>180</v>
       </c>
       <c r="F23" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>234</v>
+      </c>
+      <c r="G23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>352</v>
+        <v>301</v>
       </c>
       <c r="B24" t="s">
-        <v>208</v>
+        <v>182</v>
       </c>
       <c r="C24" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D24">
         <v>25</v>
       </c>
       <c r="F24" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>235</v>
+      </c>
+      <c r="G24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>353</v>
+        <v>302</v>
       </c>
       <c r="B25" t="s">
-        <v>209</v>
+        <v>183</v>
       </c>
       <c r="C25" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D25">
         <v>5</v>
       </c>
       <c r="F25" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>236</v>
+      </c>
+      <c r="G25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>354</v>
+        <v>303</v>
       </c>
       <c r="B26" t="s">
-        <v>210</v>
+        <v>184</v>
       </c>
       <c r="C26" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D26">
         <v>5</v>
       </c>
       <c r="F26" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>237</v>
+      </c>
+      <c r="G26">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>355</v>
+        <v>304</v>
       </c>
       <c r="B27" t="s">
-        <v>211</v>
+        <v>185</v>
       </c>
       <c r="C27" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D27">
         <v>5</v>
       </c>
       <c r="F27" t="s">
-        <v>289</v>
+        <v>238</v>
+      </c>
+      <c r="G27">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -2167,7 +2096,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2205,7 +2134,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2242,8 +2171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D42C8E0E-79CC-41C9-948F-342BD1A37C0C}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2306,7 +2235,7 @@
       </c>
       <c r="G2" s="5">
         <f ca="1">NOW()</f>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="H2">
         <v>3</v>
@@ -2333,7 +2262,7 @@
       </c>
       <c r="G3" s="5">
         <f t="shared" ref="G3:G4" ca="1" si="0">NOW()</f>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -2360,7 +2289,7 @@
       </c>
       <c r="G4" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -2383,8 +2312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978806DB-8FE4-474B-99FD-427CEAAF2910}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2426,7 +2355,7 @@
       </c>
       <c r="C2" s="6">
         <f ca="1">NOW()</f>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="2"/>
@@ -2445,7 +2374,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2489,7 +2418,7 @@
       </c>
       <c r="C2" s="6">
         <f ca="1">NOW()</f>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>71</v>
@@ -2510,7 +2439,7 @@
       </c>
       <c r="C3" s="6">
         <f ca="1">NOW()</f>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>71</v>
@@ -2531,7 +2460,7 @@
       </c>
       <c r="C4" s="6">
         <f ca="1">NOW()</f>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>71</v>
@@ -2552,7 +2481,7 @@
       </c>
       <c r="C5" s="6">
         <f ca="1">NOW()</f>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>71</v>
@@ -2575,7 +2504,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C12"/>
+      <selection activeCell="A2" sqref="A2:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2628,8 +2557,8 @@
         <v>84</v>
       </c>
       <c r="C2" s="6">
-        <f ca="1">NOW()</f>
-        <v>45747.53079837963</v>
+        <f t="shared" ref="C2:C12" ca="1" si="0">NOW()</f>
+        <v>45747.802874884263</v>
       </c>
       <c r="D2" t="s">
         <v>85</v>
@@ -2646,8 +2575,8 @@
         <v>87</v>
       </c>
       <c r="C3" s="6">
-        <f ca="1">NOW()</f>
-        <v>45747.53079837963</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>45747.802874884263</v>
       </c>
       <c r="D3" t="s">
         <v>86</v>
@@ -2664,8 +2593,8 @@
         <v>89</v>
       </c>
       <c r="C4" s="6">
-        <f ca="1">NOW()</f>
-        <v>45747.53079837963</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>45747.802874884263</v>
       </c>
       <c r="D4" t="s">
         <v>88</v>
@@ -2682,8 +2611,8 @@
         <v>80</v>
       </c>
       <c r="C5" s="6">
-        <f ca="1">NOW()</f>
-        <v>45747.53079837963</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>45747.802874884263</v>
       </c>
       <c r="D5" t="s">
         <v>90</v>
@@ -2700,8 +2629,8 @@
         <v>93</v>
       </c>
       <c r="C6" s="6">
-        <f ca="1">NOW()</f>
-        <v>45747.53079837963</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>45747.802874884263</v>
       </c>
       <c r="D6" t="s">
         <v>92</v>
@@ -2718,8 +2647,8 @@
         <v>76</v>
       </c>
       <c r="C7" s="6">
-        <f ca="1">NOW()</f>
-        <v>45747.53079837963</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>45747.802874884263</v>
       </c>
       <c r="D7" t="s">
         <v>92</v>
@@ -2736,8 +2665,8 @@
         <v>79</v>
       </c>
       <c r="C8" s="6">
-        <f ca="1">NOW()</f>
-        <v>45747.53079837963</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>45747.802874884263</v>
       </c>
       <c r="D8" t="s">
         <v>92</v>
@@ -2754,8 +2683,8 @@
         <v>78</v>
       </c>
       <c r="C9" s="6">
-        <f ca="1">NOW()</f>
-        <v>45747.53079837963</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>45747.802874884263</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -2769,8 +2698,8 @@
         <v>97</v>
       </c>
       <c r="C10" s="6">
-        <f ca="1">NOW()</f>
-        <v>45747.53079837963</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>45747.802874884263</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>94</v>
@@ -2787,8 +2716,8 @@
         <v>105</v>
       </c>
       <c r="C11" s="6">
-        <f ca="1">NOW()</f>
-        <v>45747.53079837963</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>45747.802874884263</v>
       </c>
       <c r="D11" t="s">
         <v>95</v>
@@ -2805,8 +2734,8 @@
         <v>98</v>
       </c>
       <c r="C12" s="6">
-        <f ca="1">NOW()</f>
-        <v>45747.53079837963</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>45747.802874884263</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>96</v>
@@ -2862,7 +2791,7 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D13"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15"/>
@@ -2910,7 +2839,7 @@
       </c>
       <c r="D2" s="6">
         <f ca="1">NOW()</f>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="F2">
         <v>480</v>
@@ -2929,7 +2858,7 @@
       </c>
       <c r="D3" s="6">
         <f t="shared" ref="D3:D13" ca="1" si="0">NOW()</f>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="F3">
         <v>960</v>
@@ -2948,7 +2877,7 @@
       </c>
       <c r="D4" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="F4">
         <v>480</v>
@@ -2967,7 +2896,7 @@
       </c>
       <c r="D5" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="F5">
         <v>1440</v>
@@ -2986,7 +2915,7 @@
       </c>
       <c r="D6" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -3001,7 +2930,7 @@
       </c>
       <c r="D7" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -3016,7 +2945,7 @@
       </c>
       <c r="D8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -3031,7 +2960,7 @@
       </c>
       <c r="D9" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -3046,7 +2975,7 @@
       </c>
       <c r="D10" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="E10" t="s">
         <v>99</v>
@@ -3064,7 +2993,7 @@
       </c>
       <c r="D11" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="E11" t="s">
         <v>117</v>
@@ -3082,7 +3011,7 @@
       </c>
       <c r="D12" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="E12" t="s">
         <v>118</v>
@@ -3100,7 +3029,7 @@
       </c>
       <c r="D13" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
     </row>
   </sheetData>
@@ -3112,15 +3041,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666A1DBF-4A90-426C-A8FE-B6C9014C9F32}">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView topLeftCell="A27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="40.85546875" customWidth="1"/>
     <col min="2" max="2" width="127" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="41.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="54.140625" bestFit="1" customWidth="1"/>
@@ -3163,14 +3092,14 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>237</v>
+        <v>186</v>
       </c>
       <c r="B2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C2" s="5">
         <f ca="1">NOW()</f>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D2">
         <v>50</v>
@@ -3184,20 +3113,20 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>238</v>
+        <v>187</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C3" s="5">
         <f t="shared" ref="C3:C59" ca="1" si="0">NOW()</f>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D3">
         <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>132</v>
+        <v>101</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -3205,20 +3134,20 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>239</v>
+        <v>188</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C4" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D4">
         <v>50</v>
       </c>
       <c r="E4" t="s">
-        <v>133</v>
+        <v>101</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -3226,20 +3155,20 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>240</v>
+        <v>189</v>
       </c>
       <c r="B5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C5" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D5">
         <v>50</v>
       </c>
       <c r="E5" t="s">
-        <v>134</v>
+        <v>101</v>
       </c>
       <c r="G5">
         <v>4</v>
@@ -3247,20 +3176,20 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>241</v>
+        <v>190</v>
       </c>
       <c r="B6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D6">
         <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>157</v>
+        <v>101</v>
       </c>
       <c r="G6">
         <v>5</v>
@@ -3268,20 +3197,20 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>242</v>
+        <v>191</v>
       </c>
       <c r="B7" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D7">
         <v>50</v>
       </c>
       <c r="E7" t="s">
-        <v>158</v>
+        <v>101</v>
       </c>
       <c r="G7">
         <v>6</v>
@@ -3289,20 +3218,20 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>243</v>
+        <v>192</v>
       </c>
       <c r="B8" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D8">
         <v>60</v>
       </c>
       <c r="E8" t="s">
-        <v>159</v>
+        <v>101</v>
       </c>
       <c r="G8">
         <v>7</v>
@@ -3310,20 +3239,20 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>244</v>
+        <v>193</v>
       </c>
       <c r="B9" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D9">
         <v>60</v>
       </c>
       <c r="E9" t="s">
-        <v>160</v>
+        <v>101</v>
       </c>
       <c r="G9">
         <v>8</v>
@@ -3331,20 +3260,20 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>245</v>
+        <v>194</v>
       </c>
       <c r="B10" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D10">
         <v>60</v>
       </c>
       <c r="E10" t="s">
-        <v>161</v>
+        <v>101</v>
       </c>
       <c r="G10">
         <v>9</v>
@@ -3352,20 +3281,20 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>246</v>
+        <v>195</v>
       </c>
       <c r="B11" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C11" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D11">
         <v>60</v>
       </c>
       <c r="E11" t="s">
-        <v>162</v>
+        <v>101</v>
       </c>
       <c r="G11">
         <v>10</v>
@@ -3373,20 +3302,20 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>247</v>
+        <v>196</v>
       </c>
       <c r="B12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D12">
         <v>60</v>
       </c>
       <c r="E12" t="s">
-        <v>163</v>
+        <v>101</v>
       </c>
       <c r="G12">
         <v>11</v>
@@ -3394,20 +3323,20 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>248</v>
+        <v>197</v>
       </c>
       <c r="B13" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C13" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D13">
         <v>60</v>
       </c>
       <c r="E13" t="s">
-        <v>164</v>
+        <v>101</v>
       </c>
       <c r="G13">
         <v>12</v>
@@ -3415,20 +3344,20 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>249</v>
+        <v>198</v>
       </c>
       <c r="B14" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D14">
         <v>60</v>
       </c>
       <c r="E14" t="s">
-        <v>165</v>
+        <v>101</v>
       </c>
       <c r="G14">
         <v>13</v>
@@ -3436,20 +3365,20 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>250</v>
+        <v>199</v>
       </c>
       <c r="B15" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C15" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D15">
         <v>60</v>
       </c>
       <c r="E15" t="s">
-        <v>166</v>
+        <v>101</v>
       </c>
       <c r="G15">
         <v>14</v>
@@ -3457,20 +3386,20 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>251</v>
+        <v>200</v>
       </c>
       <c r="B16" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C16" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D16">
         <v>60</v>
       </c>
       <c r="E16" t="s">
-        <v>167</v>
+        <v>101</v>
       </c>
       <c r="G16">
         <v>15</v>
@@ -3478,20 +3407,20 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>252</v>
+        <v>201</v>
       </c>
       <c r="B17" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C17" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D17">
         <v>60</v>
       </c>
       <c r="E17" t="s">
-        <v>168</v>
+        <v>101</v>
       </c>
       <c r="G17">
         <v>16</v>
@@ -3499,20 +3428,20 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>253</v>
+        <v>202</v>
       </c>
       <c r="B18" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C18" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D18">
         <v>60</v>
       </c>
       <c r="E18" t="s">
-        <v>169</v>
+        <v>101</v>
       </c>
       <c r="G18">
         <v>17</v>
@@ -3520,20 +3449,20 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>254</v>
+        <v>203</v>
       </c>
       <c r="B19" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C19" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D19">
         <v>60</v>
       </c>
       <c r="E19" t="s">
-        <v>170</v>
+        <v>101</v>
       </c>
       <c r="G19">
         <v>18</v>
@@ -3541,20 +3470,20 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>255</v>
+        <v>204</v>
       </c>
       <c r="B20" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C20" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D20">
         <v>60</v>
       </c>
       <c r="E20" t="s">
-        <v>171</v>
+        <v>101</v>
       </c>
       <c r="G20">
         <v>19</v>
@@ -3562,20 +3491,20 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>256</v>
+        <v>205</v>
       </c>
       <c r="B21" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C21" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D21">
         <v>60</v>
       </c>
       <c r="E21" t="s">
-        <v>172</v>
+        <v>101</v>
       </c>
       <c r="G21">
         <v>20</v>
@@ -3583,20 +3512,20 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>257</v>
+        <v>206</v>
       </c>
       <c r="B22" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C22" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D22">
         <v>60</v>
       </c>
       <c r="E22" t="s">
-        <v>173</v>
+        <v>101</v>
       </c>
       <c r="G22">
         <v>21</v>
@@ -3604,14 +3533,14 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>258</v>
+        <v>207</v>
       </c>
       <c r="B23" t="s">
-        <v>179</v>
+        <v>153</v>
       </c>
       <c r="C23" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D23">
         <v>1035</v>
@@ -3625,20 +3554,20 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>259</v>
+        <v>208</v>
       </c>
       <c r="B24" t="s">
-        <v>180</v>
+        <v>154</v>
       </c>
       <c r="C24" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D24">
         <v>1320</v>
       </c>
       <c r="E24" t="s">
-        <v>174</v>
+        <v>102</v>
       </c>
       <c r="G24">
         <v>2</v>
@@ -3646,20 +3575,20 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>260</v>
+        <v>209</v>
       </c>
       <c r="B25" t="s">
-        <v>181</v>
+        <v>155</v>
       </c>
       <c r="C25" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D25">
         <v>1200</v>
       </c>
       <c r="E25" t="s">
-        <v>175</v>
+        <v>102</v>
       </c>
       <c r="G25">
         <v>3</v>
@@ -3667,20 +3596,20 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>261</v>
+        <v>210</v>
       </c>
       <c r="B26" t="s">
-        <v>182</v>
+        <v>156</v>
       </c>
       <c r="C26" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D26">
         <v>1140</v>
       </c>
       <c r="E26" t="s">
-        <v>176</v>
+        <v>102</v>
       </c>
       <c r="G26">
         <v>4</v>
@@ -3688,20 +3617,20 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>262</v>
+        <v>211</v>
       </c>
       <c r="B27" t="s">
-        <v>183</v>
+        <v>157</v>
       </c>
       <c r="C27" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D27">
         <v>900</v>
       </c>
       <c r="E27" t="s">
-        <v>177</v>
+        <v>102</v>
       </c>
       <c r="G27">
         <v>5</v>
@@ -3709,20 +3638,20 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>263</v>
+        <v>212</v>
       </c>
       <c r="B28" t="s">
-        <v>184</v>
+        <v>158</v>
       </c>
       <c r="C28" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D28">
         <v>675</v>
       </c>
       <c r="E28" t="s">
-        <v>178</v>
+        <v>102</v>
       </c>
       <c r="G28">
         <v>6</v>
@@ -3730,14 +3659,14 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>264</v>
+        <v>213</v>
       </c>
       <c r="B29" t="s">
-        <v>185</v>
+        <v>159</v>
       </c>
       <c r="C29" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D29">
         <v>15</v>
@@ -3751,20 +3680,20 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>265</v>
+        <v>214</v>
       </c>
       <c r="B30" t="s">
-        <v>300</v>
+        <v>249</v>
       </c>
       <c r="C30" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D30">
         <v>40</v>
       </c>
       <c r="E30" t="s">
-        <v>212</v>
+        <v>103</v>
       </c>
       <c r="G30">
         <v>1</v>
@@ -3772,20 +3701,20 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>266</v>
+        <v>215</v>
       </c>
       <c r="B31" t="s">
-        <v>301</v>
+        <v>250</v>
       </c>
       <c r="C31" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D31">
         <v>45</v>
       </c>
       <c r="E31" t="s">
-        <v>213</v>
+        <v>103</v>
       </c>
       <c r="G31">
         <v>2</v>
@@ -3793,20 +3722,20 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>267</v>
+        <v>216</v>
       </c>
       <c r="B32" t="s">
-        <v>302</v>
+        <v>251</v>
       </c>
       <c r="C32" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D32">
         <v>130</v>
       </c>
       <c r="E32" t="s">
-        <v>214</v>
+        <v>103</v>
       </c>
       <c r="G32">
         <v>3</v>
@@ -3814,20 +3743,20 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>268</v>
+        <v>217</v>
       </c>
       <c r="B33" t="s">
-        <v>303</v>
+        <v>252</v>
       </c>
       <c r="C33" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D33">
         <v>90</v>
       </c>
       <c r="E33" t="s">
-        <v>215</v>
+        <v>103</v>
       </c>
       <c r="G33">
         <v>4</v>
@@ -3835,20 +3764,20 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>269</v>
+        <v>218</v>
       </c>
       <c r="B34" t="s">
-        <v>304</v>
+        <v>253</v>
       </c>
       <c r="C34" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D34">
         <v>120</v>
       </c>
       <c r="E34" t="s">
-        <v>216</v>
+        <v>103</v>
       </c>
       <c r="G34">
         <v>5</v>
@@ -3856,20 +3785,20 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>270</v>
+        <v>219</v>
       </c>
       <c r="B35" t="s">
-        <v>305</v>
+        <v>254</v>
       </c>
       <c r="C35" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D35">
         <v>50</v>
       </c>
       <c r="E35" t="s">
-        <v>217</v>
+        <v>103</v>
       </c>
       <c r="G35">
         <v>6</v>
@@ -3877,20 +3806,20 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>271</v>
+        <v>220</v>
       </c>
       <c r="B36" t="s">
-        <v>306</v>
+        <v>255</v>
       </c>
       <c r="C36" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D36">
         <v>25</v>
       </c>
       <c r="E36" t="s">
-        <v>218</v>
+        <v>103</v>
       </c>
       <c r="G36">
         <v>7</v>
@@ -3898,20 +3827,20 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>272</v>
+        <v>221</v>
       </c>
       <c r="B37" t="s">
-        <v>307</v>
+        <v>256</v>
       </c>
       <c r="C37" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D37">
         <v>40</v>
       </c>
       <c r="E37" t="s">
-        <v>219</v>
+        <v>103</v>
       </c>
       <c r="G37">
         <v>8</v>
@@ -3919,20 +3848,20 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>273</v>
+        <v>222</v>
       </c>
       <c r="B38" t="s">
-        <v>308</v>
+        <v>257</v>
       </c>
       <c r="C38" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D38">
         <v>50</v>
       </c>
       <c r="E38" t="s">
-        <v>220</v>
+        <v>103</v>
       </c>
       <c r="G38">
         <v>9</v>
@@ -3940,20 +3869,20 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>274</v>
+        <v>223</v>
       </c>
       <c r="B39" t="s">
-        <v>309</v>
+        <v>258</v>
       </c>
       <c r="C39" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D39">
         <v>40</v>
       </c>
       <c r="E39" t="s">
-        <v>221</v>
+        <v>103</v>
       </c>
       <c r="G39">
         <v>10</v>
@@ -3961,20 +3890,20 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>275</v>
+        <v>224</v>
       </c>
       <c r="B40" t="s">
-        <v>310</v>
+        <v>259</v>
       </c>
       <c r="C40" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D40">
         <v>80</v>
       </c>
       <c r="E40" t="s">
-        <v>222</v>
+        <v>103</v>
       </c>
       <c r="G40">
         <v>11</v>
@@ -3982,20 +3911,20 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>276</v>
+        <v>225</v>
       </c>
       <c r="B41" t="s">
-        <v>311</v>
+        <v>260</v>
       </c>
       <c r="C41" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D41">
         <v>40</v>
       </c>
       <c r="E41" t="s">
-        <v>223</v>
+        <v>103</v>
       </c>
       <c r="G41">
         <v>12</v>
@@ -4003,20 +3932,20 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>277</v>
+        <v>226</v>
       </c>
       <c r="B42" t="s">
-        <v>312</v>
+        <v>261</v>
       </c>
       <c r="C42" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D42">
         <v>270</v>
       </c>
       <c r="E42" t="s">
-        <v>224</v>
+        <v>103</v>
       </c>
       <c r="G42">
         <v>13</v>
@@ -4024,20 +3953,20 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>278</v>
+        <v>227</v>
       </c>
       <c r="B43" t="s">
-        <v>313</v>
+        <v>262</v>
       </c>
       <c r="C43" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D43">
         <v>210</v>
       </c>
       <c r="E43" t="s">
-        <v>225</v>
+        <v>103</v>
       </c>
       <c r="G43">
         <v>14</v>
@@ -4045,20 +3974,20 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>279</v>
+        <v>228</v>
       </c>
       <c r="B44" t="s">
-        <v>314</v>
+        <v>263</v>
       </c>
       <c r="C44" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D44">
         <v>170</v>
       </c>
       <c r="E44" t="s">
-        <v>226</v>
+        <v>103</v>
       </c>
       <c r="G44">
         <v>15</v>
@@ -4066,20 +3995,20 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>280</v>
+        <v>229</v>
       </c>
       <c r="B45" t="s">
-        <v>315</v>
+        <v>264</v>
       </c>
       <c r="C45" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D45">
         <v>40</v>
       </c>
       <c r="E45" t="s">
-        <v>227</v>
+        <v>103</v>
       </c>
       <c r="G45">
         <v>16</v>
@@ -4087,20 +4016,20 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>281</v>
+        <v>230</v>
       </c>
       <c r="B46" t="s">
-        <v>316</v>
+        <v>265</v>
       </c>
       <c r="C46" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D46">
         <v>35</v>
       </c>
       <c r="E46" t="s">
-        <v>228</v>
+        <v>103</v>
       </c>
       <c r="G46">
         <v>17</v>
@@ -4108,20 +4037,20 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>282</v>
+        <v>231</v>
       </c>
       <c r="B47" t="s">
-        <v>317</v>
+        <v>266</v>
       </c>
       <c r="C47" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D47">
         <v>40</v>
       </c>
       <c r="E47" t="s">
-        <v>229</v>
+        <v>103</v>
       </c>
       <c r="G47">
         <v>18</v>
@@ -4129,20 +4058,20 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>283</v>
+        <v>232</v>
       </c>
       <c r="B48" t="s">
-        <v>318</v>
+        <v>267</v>
       </c>
       <c r="C48" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D48">
         <v>110</v>
       </c>
       <c r="E48" t="s">
-        <v>230</v>
+        <v>103</v>
       </c>
       <c r="G48">
         <v>19</v>
@@ -4150,20 +4079,20 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>284</v>
+        <v>233</v>
       </c>
       <c r="B49" t="s">
-        <v>319</v>
+        <v>268</v>
       </c>
       <c r="C49" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D49">
         <v>70</v>
       </c>
       <c r="E49" t="s">
-        <v>231</v>
+        <v>103</v>
       </c>
       <c r="G49">
         <v>20</v>
@@ -4171,20 +4100,20 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>285</v>
+        <v>234</v>
       </c>
       <c r="B50" t="s">
-        <v>320</v>
+        <v>269</v>
       </c>
       <c r="C50" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D50">
         <v>370</v>
       </c>
       <c r="E50" t="s">
-        <v>232</v>
+        <v>103</v>
       </c>
       <c r="G50">
         <v>21</v>
@@ -4192,20 +4121,20 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>286</v>
+        <v>235</v>
       </c>
       <c r="B51" t="s">
-        <v>321</v>
+        <v>270</v>
       </c>
       <c r="C51" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D51">
         <v>30</v>
       </c>
       <c r="E51" t="s">
-        <v>233</v>
+        <v>103</v>
       </c>
       <c r="G51">
         <v>22</v>
@@ -4213,20 +4142,20 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>287</v>
+        <v>236</v>
       </c>
       <c r="B52" t="s">
-        <v>322</v>
+        <v>271</v>
       </c>
       <c r="C52" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D52">
         <v>120</v>
       </c>
       <c r="E52" t="s">
-        <v>234</v>
+        <v>103</v>
       </c>
       <c r="G52">
         <v>23</v>
@@ -4234,20 +4163,20 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>288</v>
+        <v>237</v>
       </c>
       <c r="B53" t="s">
-        <v>323</v>
+        <v>272</v>
       </c>
       <c r="C53" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D53">
         <v>130</v>
       </c>
       <c r="E53" t="s">
-        <v>235</v>
+        <v>103</v>
       </c>
       <c r="G53">
         <v>24</v>
@@ -4255,20 +4184,20 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
-        <v>289</v>
+        <v>238</v>
       </c>
       <c r="B54" t="s">
-        <v>324</v>
+        <v>273</v>
       </c>
       <c r="C54" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D54">
         <v>120</v>
       </c>
       <c r="E54" t="s">
-        <v>236</v>
+        <v>103</v>
       </c>
       <c r="G54">
         <v>25</v>
@@ -4276,14 +4205,14 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>290</v>
+        <v>239</v>
       </c>
       <c r="B55" t="s">
-        <v>325</v>
+        <v>274</v>
       </c>
       <c r="C55" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D55">
         <v>480</v>
@@ -4292,7 +4221,7 @@
         <v>104</v>
       </c>
       <c r="F55" t="s">
-        <v>295</v>
+        <v>244</v>
       </c>
       <c r="G55">
         <v>1</v>
@@ -4300,14 +4229,14 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>291</v>
+        <v>240</v>
       </c>
       <c r="B56" t="s">
-        <v>326</v>
+        <v>275</v>
       </c>
       <c r="C56" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D56">
         <v>960</v>
@@ -4316,7 +4245,7 @@
         <v>104</v>
       </c>
       <c r="F56" t="s">
-        <v>296</v>
+        <v>245</v>
       </c>
       <c r="G56">
         <v>2</v>
@@ -4324,14 +4253,14 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>292</v>
+        <v>241</v>
       </c>
       <c r="B57" t="s">
-        <v>327</v>
+        <v>276</v>
       </c>
       <c r="C57" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D57">
         <v>960</v>
@@ -4340,7 +4269,7 @@
         <v>104</v>
       </c>
       <c r="F57" t="s">
-        <v>297</v>
+        <v>246</v>
       </c>
       <c r="G57">
         <v>3</v>
@@ -4348,14 +4277,14 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>293</v>
+        <v>242</v>
       </c>
       <c r="B58" t="s">
-        <v>328</v>
+        <v>277</v>
       </c>
       <c r="C58" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D58">
         <v>1920</v>
@@ -4364,7 +4293,7 @@
         <v>104</v>
       </c>
       <c r="F58" t="s">
-        <v>298</v>
+        <v>247</v>
       </c>
       <c r="G58">
         <v>4</v>
@@ -4372,14 +4301,14 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>294</v>
+        <v>243</v>
       </c>
       <c r="B59" t="s">
-        <v>329</v>
+        <v>278</v>
       </c>
       <c r="C59" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45747.53079837963</v>
+        <v>45747.802874884263</v>
       </c>
       <c r="D59">
         <v>1440</v>
@@ -4388,7 +4317,7 @@
         <v>104</v>
       </c>
       <c r="F59" t="s">
-        <v>299</v>
+        <v>248</v>
       </c>
       <c r="G59">
         <v>5</v>

</xml_diff>

<commit_message>
feate: update registration method
</commit_message>
<xml_diff>
--- a/database/data_for_import/data_for_import.xlsx
+++ b/database/data_for_import/data_for_import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Progect\pp+diplom\study_1c\database\data_for_import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E531030-C3B2-4E32-8438-B82B4CF3674B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DEF496-F34E-4B15-940A-A5DA4B283366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" tabRatio="775" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4305" yWindow="1800" windowWidth="18900" windowHeight="10965" tabRatio="775" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="roles" sheetId="1" r:id="rId1"/>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="C2" s="5">
         <f ca="1">NOW()</f>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D2">
         <v>50</v>
@@ -1516,7 +1516,7 @@
       </c>
       <c r="C3" s="5">
         <f t="shared" ref="C3:C59" ca="1" si="0">NOW()</f>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D3">
         <v>50</v>
@@ -1537,7 +1537,7 @@
       </c>
       <c r="C4" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D4">
         <v>50</v>
@@ -1558,7 +1558,7 @@
       </c>
       <c r="C5" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D5">
         <v>50</v>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="C6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D6">
         <v>50</v>
@@ -1600,7 +1600,7 @@
       </c>
       <c r="C7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D7">
         <v>50</v>
@@ -1621,7 +1621,7 @@
       </c>
       <c r="C8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D8">
         <v>60</v>
@@ -1642,7 +1642,7 @@
       </c>
       <c r="C9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D9">
         <v>60</v>
@@ -1663,7 +1663,7 @@
       </c>
       <c r="C10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D10">
         <v>60</v>
@@ -1684,7 +1684,7 @@
       </c>
       <c r="C11" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D11">
         <v>60</v>
@@ -1705,7 +1705,7 @@
       </c>
       <c r="C12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D12">
         <v>60</v>
@@ -1726,7 +1726,7 @@
       </c>
       <c r="C13" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D13">
         <v>60</v>
@@ -1747,7 +1747,7 @@
       </c>
       <c r="C14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D14">
         <v>60</v>
@@ -1768,7 +1768,7 @@
       </c>
       <c r="C15" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D15">
         <v>60</v>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="C16" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D16">
         <v>60</v>
@@ -1810,7 +1810,7 @@
       </c>
       <c r="C17" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D17">
         <v>60</v>
@@ -1831,7 +1831,7 @@
       </c>
       <c r="C18" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D18">
         <v>60</v>
@@ -1852,7 +1852,7 @@
       </c>
       <c r="C19" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D19">
         <v>60</v>
@@ -1873,7 +1873,7 @@
       </c>
       <c r="C20" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D20">
         <v>60</v>
@@ -1894,7 +1894,7 @@
       </c>
       <c r="C21" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D21">
         <v>60</v>
@@ -1915,7 +1915,7 @@
       </c>
       <c r="C22" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D22">
         <v>60</v>
@@ -1936,7 +1936,7 @@
       </c>
       <c r="C23" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D23">
         <v>1035</v>
@@ -1957,7 +1957,7 @@
       </c>
       <c r="C24" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D24">
         <v>1320</v>
@@ -1978,7 +1978,7 @@
       </c>
       <c r="C25" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D25">
         <v>1200</v>
@@ -1999,7 +1999,7 @@
       </c>
       <c r="C26" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D26">
         <v>1140</v>
@@ -2020,7 +2020,7 @@
       </c>
       <c r="C27" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D27">
         <v>900</v>
@@ -2041,7 +2041,7 @@
       </c>
       <c r="C28" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D28">
         <v>675</v>
@@ -2062,7 +2062,7 @@
       </c>
       <c r="C29" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D29">
         <v>15</v>
@@ -2083,7 +2083,7 @@
       </c>
       <c r="C30" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D30">
         <v>40</v>
@@ -2104,7 +2104,7 @@
       </c>
       <c r="C31" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D31">
         <v>45</v>
@@ -2125,7 +2125,7 @@
       </c>
       <c r="C32" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D32">
         <v>130</v>
@@ -2146,7 +2146,7 @@
       </c>
       <c r="C33" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D33">
         <v>90</v>
@@ -2167,7 +2167,7 @@
       </c>
       <c r="C34" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D34">
         <v>120</v>
@@ -2188,7 +2188,7 @@
       </c>
       <c r="C35" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D35">
         <v>50</v>
@@ -2209,7 +2209,7 @@
       </c>
       <c r="C36" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D36">
         <v>25</v>
@@ -2230,7 +2230,7 @@
       </c>
       <c r="C37" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D37">
         <v>40</v>
@@ -2251,7 +2251,7 @@
       </c>
       <c r="C38" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D38">
         <v>50</v>
@@ -2272,7 +2272,7 @@
       </c>
       <c r="C39" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D39">
         <v>40</v>
@@ -2293,7 +2293,7 @@
       </c>
       <c r="C40" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D40">
         <v>80</v>
@@ -2314,7 +2314,7 @@
       </c>
       <c r="C41" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D41">
         <v>40</v>
@@ -2335,7 +2335,7 @@
       </c>
       <c r="C42" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D42">
         <v>270</v>
@@ -2356,7 +2356,7 @@
       </c>
       <c r="C43" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D43">
         <v>210</v>
@@ -2377,7 +2377,7 @@
       </c>
       <c r="C44" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D44">
         <v>170</v>
@@ -2398,7 +2398,7 @@
       </c>
       <c r="C45" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D45">
         <v>40</v>
@@ -2419,7 +2419,7 @@
       </c>
       <c r="C46" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D46">
         <v>35</v>
@@ -2440,7 +2440,7 @@
       </c>
       <c r="C47" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D47">
         <v>40</v>
@@ -2461,7 +2461,7 @@
       </c>
       <c r="C48" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D48">
         <v>110</v>
@@ -2482,7 +2482,7 @@
       </c>
       <c r="C49" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D49">
         <v>70</v>
@@ -2503,7 +2503,7 @@
       </c>
       <c r="C50" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D50">
         <v>370</v>
@@ -2524,7 +2524,7 @@
       </c>
       <c r="C51" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D51">
         <v>30</v>
@@ -2545,7 +2545,7 @@
       </c>
       <c r="C52" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D52">
         <v>120</v>
@@ -2566,7 +2566,7 @@
       </c>
       <c r="C53" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D53">
         <v>130</v>
@@ -2587,7 +2587,7 @@
       </c>
       <c r="C54" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D54">
         <v>120</v>
@@ -2608,7 +2608,7 @@
       </c>
       <c r="C55" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D55">
         <v>480</v>
@@ -2632,7 +2632,7 @@
       </c>
       <c r="C56" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D56">
         <v>960</v>
@@ -2656,7 +2656,7 @@
       </c>
       <c r="C57" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D57">
         <v>960</v>
@@ -2680,7 +2680,7 @@
       </c>
       <c r="C58" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D58">
         <v>1920</v>
@@ -2704,7 +2704,7 @@
       </c>
       <c r="C59" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D59">
         <v>1440</v>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="C2" s="5">
         <f t="shared" ref="C2:C27" ca="1" si="0">NOW()</f>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D2">
         <v>5</v>
@@ -2802,7 +2802,7 @@
       </c>
       <c r="C3" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D3">
         <v>20</v>
@@ -2823,7 +2823,7 @@
       </c>
       <c r="C4" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D4">
         <v>25</v>
@@ -2844,7 +2844,7 @@
       </c>
       <c r="C5" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D5">
         <v>120</v>
@@ -2865,7 +2865,7 @@
       </c>
       <c r="C6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D6">
         <v>60</v>
@@ -2886,7 +2886,7 @@
       </c>
       <c r="C7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -2907,7 +2907,7 @@
       </c>
       <c r="C8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D8">
         <v>25</v>
@@ -2928,7 +2928,7 @@
       </c>
       <c r="C9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D9">
         <v>15</v>
@@ -2949,7 +2949,7 @@
       </c>
       <c r="C10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D10">
         <v>25</v>
@@ -2970,7 +2970,7 @@
       </c>
       <c r="C11" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D11">
         <v>25</v>
@@ -2991,7 +2991,7 @@
       </c>
       <c r="C12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D12">
         <v>25</v>
@@ -3012,7 +3012,7 @@
       </c>
       <c r="C13" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D13">
         <v>40</v>
@@ -3033,7 +3033,7 @@
       </c>
       <c r="C14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D14">
         <v>25</v>
@@ -3054,7 +3054,7 @@
       </c>
       <c r="C15" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D15">
         <v>90</v>
@@ -3075,7 +3075,7 @@
       </c>
       <c r="C16" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D16">
         <v>90</v>
@@ -3096,7 +3096,7 @@
       </c>
       <c r="C17" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D17">
         <v>5</v>
@@ -3117,7 +3117,7 @@
       </c>
       <c r="C18" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D18">
         <v>5</v>
@@ -3138,7 +3138,7 @@
       </c>
       <c r="C19" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D19">
         <v>90</v>
@@ -3159,7 +3159,7 @@
       </c>
       <c r="C20" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D20">
         <v>25</v>
@@ -3180,7 +3180,7 @@
       </c>
       <c r="C21" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D21">
         <v>120</v>
@@ -3201,7 +3201,7 @@
       </c>
       <c r="C22" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D22">
         <v>50</v>
@@ -3222,7 +3222,7 @@
       </c>
       <c r="C23" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D23">
         <v>180</v>
@@ -3243,7 +3243,7 @@
       </c>
       <c r="C24" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D24">
         <v>25</v>
@@ -3264,7 +3264,7 @@
       </c>
       <c r="C25" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D25">
         <v>5</v>
@@ -3285,7 +3285,7 @@
       </c>
       <c r="C26" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D26">
         <v>5</v>
@@ -3306,7 +3306,7 @@
       </c>
       <c r="C27" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D27">
         <v>5</v>
@@ -3485,10 +3485,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D42C8E0E-79CC-41C9-948F-342BD1A37C0C}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3583,8 +3583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD7B66B1-6BC6-4C30-9443-0722E61BBB20}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3731,7 +3731,7 @@
       </c>
       <c r="C2" s="6">
         <f ca="1">NOW()</f>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="2"/>
@@ -3794,7 +3794,7 @@
       </c>
       <c r="C2" s="6">
         <f ca="1">NOW()</f>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>67</v>
@@ -3815,7 +3815,7 @@
       </c>
       <c r="C3" s="6">
         <f ca="1">NOW()</f>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>67</v>
@@ -3836,7 +3836,7 @@
       </c>
       <c r="C4" s="6">
         <f ca="1">NOW()</f>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>67</v>
@@ -3857,7 +3857,7 @@
       </c>
       <c r="C5" s="6">
         <f ca="1">NOW()</f>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>67</v>
@@ -3934,7 +3934,7 @@
       </c>
       <c r="C2" s="6">
         <f t="shared" ref="C2:C12" ca="1" si="0">NOW()</f>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D2" t="s">
         <v>81</v>
@@ -3952,7 +3952,7 @@
       </c>
       <c r="C3" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D3" t="s">
         <v>82</v>
@@ -3970,7 +3970,7 @@
       </c>
       <c r="C4" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
@@ -3988,7 +3988,7 @@
       </c>
       <c r="C5" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D5" t="s">
         <v>86</v>
@@ -4006,7 +4006,7 @@
       </c>
       <c r="C6" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D6" t="s">
         <v>88</v>
@@ -4024,7 +4024,7 @@
       </c>
       <c r="C7" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D7" t="s">
         <v>88</v>
@@ -4042,7 +4042,7 @@
       </c>
       <c r="C8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D8" t="s">
         <v>88</v>
@@ -4060,7 +4060,7 @@
       </c>
       <c r="C9" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -4075,7 +4075,7 @@
       </c>
       <c r="C10" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>90</v>
@@ -4093,7 +4093,7 @@
       </c>
       <c r="C11" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D11" t="s">
         <v>91</v>
@@ -4111,7 +4111,7 @@
       </c>
       <c r="C12" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>92</v>
@@ -4215,7 +4215,7 @@
       </c>
       <c r="D2" s="6">
         <f ca="1">NOW()</f>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="F2">
         <v>480</v>
@@ -4234,7 +4234,7 @@
       </c>
       <c r="D3" s="6">
         <f t="shared" ref="D3:D13" ca="1" si="0">NOW()</f>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="F3">
         <v>960</v>
@@ -4253,7 +4253,7 @@
       </c>
       <c r="D4" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="F4">
         <v>480</v>
@@ -4272,7 +4272,7 @@
       </c>
       <c r="D5" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="F5">
         <v>1440</v>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="D6" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -4306,7 +4306,7 @@
       </c>
       <c r="D7" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -4321,7 +4321,7 @@
       </c>
       <c r="D8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -4336,7 +4336,7 @@
       </c>
       <c r="D9" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -4351,7 +4351,7 @@
       </c>
       <c r="D10" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="E10" t="s">
         <v>95</v>
@@ -4369,7 +4369,7 @@
       </c>
       <c r="D11" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="E11" t="s">
         <v>113</v>
@@ -4387,7 +4387,7 @@
       </c>
       <c r="D12" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
       <c r="E12" t="s">
         <v>114</v>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="D13" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45751.564742592593</v>
+        <v>45754.005903703706</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: end creatin manage account controller
</commit_message>
<xml_diff>
--- a/database/data_for_import/data_for_import.xlsx
+++ b/database/data_for_import/data_for_import.xlsx
@@ -5,26 +5,28 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Progect\pp+diplom\study_1c\database\data_for_import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Progects\study_1c\database\data_for_import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DEF496-F34E-4B15-940A-A5DA4B283366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB11441F-061D-48B2-9F4F-AA08C34C10A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4305" yWindow="1800" windowWidth="18900" windowHeight="10965" tabRatio="775" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="775" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="roles" sheetId="1" r:id="rId1"/>
     <sheet name="material_type" sheetId="2" r:id="rId2"/>
     <sheet name="study_states" sheetId="3" r:id="rId3"/>
-    <sheet name="profile" sheetId="4" r:id="rId4"/>
-    <sheet name="auth_user" sheetId="12" r:id="rId5"/>
-    <sheet name="courses" sheetId="5" r:id="rId6"/>
-    <sheet name="courses_blocks" sheetId="6" r:id="rId7"/>
-    <sheet name="materials" sheetId="7" r:id="rId8"/>
-    <sheet name="blocks_materials" sheetId="8" r:id="rId9"/>
-    <sheet name="blocks_tasks" sheetId="9" r:id="rId10"/>
-    <sheet name="tasks_practice" sheetId="10" r:id="rId11"/>
-    <sheet name="users_tasks" sheetId="11" r:id="rId12"/>
+    <sheet name="auth_user" sheetId="12" r:id="rId4"/>
+    <sheet name="user_roles" sheetId="13" r:id="rId5"/>
+    <sheet name="profile" sheetId="4" r:id="rId6"/>
+    <sheet name="courses" sheetId="5" r:id="rId7"/>
+    <sheet name="users_courses" sheetId="14" r:id="rId8"/>
+    <sheet name="courses_blocks" sheetId="6" r:id="rId9"/>
+    <sheet name="materials" sheetId="7" r:id="rId10"/>
+    <sheet name="blocks_materials" sheetId="8" r:id="rId11"/>
+    <sheet name="blocks_tasks" sheetId="9" r:id="rId12"/>
+    <sheet name="tasks_practice" sheetId="10" r:id="rId13"/>
+    <sheet name="users_tasks" sheetId="11" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,13 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="310">
-  <si>
-    <t>role_id</t>
-  </si>
-  <si>
-    <t>role_name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="339">
   <si>
     <t>Ученик</t>
   </si>
@@ -89,55 +85,19 @@
     <t>Изучил</t>
   </si>
   <si>
-    <t>user_id</t>
-  </si>
-  <si>
     <t>user_surname</t>
   </si>
   <si>
     <t>user_name</t>
   </si>
   <si>
-    <t>user_patronymic</t>
-  </si>
-  <si>
-    <t>is_first</t>
-  </si>
-  <si>
-    <t>F45D2396-3E72-4EC7-B892-7BD454248158</t>
-  </si>
-  <si>
-    <t>060BD96A-4FC6-40F1-90A9-C2575C852868</t>
-  </si>
-  <si>
-    <t>C202E6F1-73C7-4557-907F-2EEC4D18C9FC</t>
-  </si>
-  <si>
     <t>admin@admin.com</t>
   </si>
   <si>
     <t>curator@curator.com</t>
   </si>
   <si>
-    <t>student</t>
-  </si>
-  <si>
-    <t>student@student.com</t>
-  </si>
-  <si>
     <t>admin</t>
-  </si>
-  <si>
-    <t>curator</t>
-  </si>
-  <si>
-    <t>21232f297a57a5a743894a0e4a801fc3</t>
-  </si>
-  <si>
-    <t>8a08422b4ca8a0ab0f443628d627c96b</t>
-  </si>
-  <si>
-    <t>cd73502828457d15655bbd7a63fb0bc8</t>
   </si>
   <si>
     <t>true</t>
@@ -993,28 +953,157 @@
     <t>number_practice_of_task</t>
   </si>
   <si>
-    <t>login</t>
-  </si>
-  <si>
-    <t>hash_password</t>
-  </si>
-  <si>
-    <t>data_create</t>
-  </si>
-  <si>
-    <t>role</t>
-  </si>
-  <si>
-    <t>profile_id</t>
-  </si>
-  <si>
-    <t>550e8400-e29b-41d4-a716-446655440000</t>
-  </si>
-  <si>
-    <t>a1b2c3d4-e5f6-4a7b-8c9d-0e1f2a3b4c5d</t>
-  </si>
-  <si>
     <t>f47ac10b-58cc-4372-a567-0e02b2c3d479</t>
+  </si>
+  <si>
+    <t>33b58484-1bf5-4c42-ba72-2a53bbf67581</t>
+  </si>
+  <si>
+    <t>c9eb182b-1c3e-4c3b-8c3e-1c3e4c3b8c3e</t>
+  </si>
+  <si>
+    <t>f45d2396-3e72-4ec7-b892-7bd454248158</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>IsNonManipulate</t>
+  </si>
+  <si>
+    <t>NormalizedName</t>
+  </si>
+  <si>
+    <t>ConcurrencyStamp</t>
+  </si>
+  <si>
+    <t>УЧЕНИК</t>
+  </si>
+  <si>
+    <t>КУРАТОР</t>
+  </si>
+  <si>
+    <t>АДМИНИСТРАТОР</t>
+  </si>
+  <si>
+    <t>ld</t>
+  </si>
+  <si>
+    <t>UserDataCreate</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>NormalizedUserName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>NormalizedEmail</t>
+  </si>
+  <si>
+    <t>EmailConfirmed</t>
+  </si>
+  <si>
+    <t>PasswordHash</t>
+  </si>
+  <si>
+    <t>SecurityStamp</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>PhoneNumberConfirmed</t>
+  </si>
+  <si>
+    <t>TwoFactorEnabled</t>
+  </si>
+  <si>
+    <t>LockoutEnd</t>
+  </si>
+  <si>
+    <t>LockoutEnabled</t>
+  </si>
+  <si>
+    <t>AccessFailedCount</t>
+  </si>
+  <si>
+    <t>ADMIN@ADMIN.COM</t>
+  </si>
+  <si>
+    <t>CURATOR@CURATOR.COM</t>
+  </si>
+  <si>
+    <t>AQAAAAIAAYagAAAAEDAflT7y8miLvkMRoQzUwPtEZdPNY4F6ovKJDKCWpOnEfbr8CDDrjFXVU/gkUawR5w==</t>
+  </si>
+  <si>
+    <t>AQAAAAIAAYagAAAAEP8gLY3ZDpJUkVmA9i24FRQJqYV2IMHE4trRtAqfrXTuIEcen53v8gC3TW/2/Mj8Mg==</t>
+  </si>
+  <si>
+    <t>AQAAAAIAAYagAAAAEC7EMsSEFpAz+jwGrhx54/1ovW5n8ayWd7n6e6uTmxGL7ypIUb8uekL5vdDp1hfO5w==</t>
+  </si>
+  <si>
+    <t>CJQGS6WHCU7GUHDG7VQF56UU6YK2YL4W</t>
+  </si>
+  <si>
+    <t>3C2KGRQ3OCITZBJ4UEXFHBUTB334224T</t>
+  </si>
+  <si>
+    <t>ZSI2KJLOBM4G25472UPH46K3VSVYX4EW</t>
+  </si>
+  <si>
+    <t>4c125882-5b6f-44bd-b7ed-b7aceb40d048</t>
+  </si>
+  <si>
+    <t>60d4ef1d-ebf6-4ade-81e4-d76d7bfd9311</t>
+  </si>
+  <si>
+    <t>Userld</t>
+  </si>
+  <si>
+    <t>Roleld</t>
+  </si>
+  <si>
+    <t>0196125a-2c3e-7bc4-8dd4-5eeeff3ebc2b</t>
+  </si>
+  <si>
+    <t>019612aa-c914-7445-82d7-e451806895bb</t>
+  </si>
+  <si>
+    <t>ADMIN</t>
+  </si>
+  <si>
+    <t>user@example.com</t>
+  </si>
+  <si>
+    <t>USER@EXAMPLE.COM</t>
+  </si>
+  <si>
+    <t>4c79814b-cc5b-4676-b03e-243e1451caea</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>is first</t>
+  </si>
+  <si>
+    <t>user_ld</t>
+  </si>
+  <si>
+    <t>user_ patronymic</t>
+  </si>
+  <si>
+    <t>Courseld</t>
+  </si>
+  <si>
+    <t>cu_id</t>
   </si>
 </sst>
 </file>
@@ -1394,38 +1483,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>290</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="B2" t="s">
+      <c r="D3" t="s">
+        <v>298</v>
+      </c>
+      <c r="E3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>291</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="B4" t="s">
-        <v>4</v>
+      <c r="D4" t="s">
+        <v>299</v>
+      </c>
+      <c r="E4" t="s">
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -1434,10 +1571,548 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7122162C-AD73-4663-9975-8D7C83047E49}">
+  <dimension ref="A1:F29"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="84.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="122.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="6">
+        <f t="shared" ref="C2:C12" ca="1" si="0">NOW()</f>
+        <v>45755.53341689815</v>
+      </c>
+      <c r="D2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>45755.53341689815</v>
+      </c>
+      <c r="D3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>45755.53341689815</v>
+      </c>
+      <c r="D4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>45755.53341689815</v>
+      </c>
+      <c r="D5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>45755.53341689815</v>
+      </c>
+      <c r="D6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>45755.53341689815</v>
+      </c>
+      <c r="D7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>45755.53341689815</v>
+      </c>
+      <c r="D8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>45755.53341689815</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>45755.53341689815</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>45755.53341689815</v>
+      </c>
+      <c r="D11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>45755.53341689815</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" s="4"/>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="4"/>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="4"/>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="4"/>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" s="4"/>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="4"/>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" s="4"/>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" s="4"/>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" s="4"/>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" s="4"/>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29" s="4"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D10" r:id="rId1" xr:uid="{223B1678-144B-4D76-9D65-D27BD252BBF2}"/>
+    <hyperlink ref="D12" r:id="rId2" xr:uid="{C6D3A5D0-19B9-49D5-A5EE-452D74ABD85D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5370AC90-9927-445C-B04F-4A41A0706261}">
+  <dimension ref="A1:O13"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="69.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="33" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="62.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="6">
+        <f ca="1">NOW()</f>
+        <v>45755.53341689815</v>
+      </c>
+      <c r="F2">
+        <v>480</v>
+      </c>
+      <c r="O2" s="2"/>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="6">
+        <f t="shared" ref="D3:D13" ca="1" si="0">NOW()</f>
+        <v>45755.53341689815</v>
+      </c>
+      <c r="F3">
+        <v>960</v>
+      </c>
+      <c r="O3" s="2"/>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>45755.53341689815</v>
+      </c>
+      <c r="F4">
+        <v>480</v>
+      </c>
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>45755.53341689815</v>
+      </c>
+      <c r="F5">
+        <v>1440</v>
+      </c>
+      <c r="O5" s="2"/>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>45755.53341689815</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>45755.53341689815</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>45755.53341689815</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>45755.53341689815</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>45755.53341689815</v>
+      </c>
+      <c r="E10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>45755.53341689815</v>
+      </c>
+      <c r="E11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>45755.53341689815</v>
+      </c>
+      <c r="E12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>45755.53341689815</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666A1DBF-4A90-426C-A8FE-B6C9014C9F32}">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A44" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:H59"/>
     </sheetView>
   </sheetViews>
@@ -1462,46 +2137,46 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="E1" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="G1" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="H1" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="C2" s="5">
         <f ca="1">NOW()</f>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D2">
         <v>50</v>
       </c>
       <c r="E2" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -1509,20 +2184,20 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="B3" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="C3" s="5">
         <f t="shared" ref="C3:C59" ca="1" si="0">NOW()</f>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D3">
         <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -1530,20 +2205,20 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="B4" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="C4" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D4">
         <v>50</v>
       </c>
       <c r="E4" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -1551,20 +2226,20 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B5" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="C5" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D5">
         <v>50</v>
       </c>
       <c r="E5" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="G5">
         <v>4</v>
@@ -1572,20 +2247,20 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="B6" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="C6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D6">
         <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="G6">
         <v>5</v>
@@ -1593,20 +2268,20 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="B7" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="C7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D7">
         <v>50</v>
       </c>
       <c r="E7" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="G7">
         <v>6</v>
@@ -1614,20 +2289,20 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="B8" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="C8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D8">
         <v>60</v>
       </c>
       <c r="E8" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="G8">
         <v>7</v>
@@ -1635,20 +2310,20 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="B9" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="C9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D9">
         <v>60</v>
       </c>
       <c r="E9" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="G9">
         <v>8</v>
@@ -1656,20 +2331,20 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="B10" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="C10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D10">
         <v>60</v>
       </c>
       <c r="E10" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="G10">
         <v>9</v>
@@ -1677,20 +2352,20 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="B11" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="C11" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D11">
         <v>60</v>
       </c>
       <c r="E11" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="G11">
         <v>10</v>
@@ -1698,20 +2373,20 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="B12" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="C12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D12">
         <v>60</v>
       </c>
       <c r="E12" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="G12">
         <v>11</v>
@@ -1719,20 +2394,20 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="B13" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="C13" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D13">
         <v>60</v>
       </c>
       <c r="E13" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="G13">
         <v>12</v>
@@ -1740,20 +2415,20 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="B14" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="C14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D14">
         <v>60</v>
       </c>
       <c r="E14" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="G14">
         <v>13</v>
@@ -1761,20 +2436,20 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="B15" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="C15" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D15">
         <v>60</v>
       </c>
       <c r="E15" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="G15">
         <v>14</v>
@@ -1782,20 +2457,20 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="B16" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="C16" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D16">
         <v>60</v>
       </c>
       <c r="E16" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="G16">
         <v>15</v>
@@ -1803,20 +2478,20 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="B17" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="C17" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D17">
         <v>60</v>
       </c>
       <c r="E17" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="G17">
         <v>16</v>
@@ -1824,20 +2499,20 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="B18" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="C18" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D18">
         <v>60</v>
       </c>
       <c r="E18" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="G18">
         <v>17</v>
@@ -1845,20 +2520,20 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="B19" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="C19" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D19">
         <v>60</v>
       </c>
       <c r="E19" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="G19">
         <v>18</v>
@@ -1866,20 +2541,20 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="B20" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="C20" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D20">
         <v>60</v>
       </c>
       <c r="E20" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="G20">
         <v>19</v>
@@ -1887,20 +2562,20 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="B21" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="C21" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D21">
         <v>60</v>
       </c>
       <c r="E21" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="G21">
         <v>20</v>
@@ -1908,20 +2583,20 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="B22" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="C22" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D22">
         <v>60</v>
       </c>
       <c r="E22" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="G22">
         <v>21</v>
@@ -1929,20 +2604,20 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="B23" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="C23" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D23">
         <v>1035</v>
       </c>
       <c r="E23" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -1950,20 +2625,20 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="B24" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="C24" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D24">
         <v>1320</v>
       </c>
       <c r="E24" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="G24">
         <v>2</v>
@@ -1971,20 +2646,20 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="B25" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="C25" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D25">
         <v>1200</v>
       </c>
       <c r="E25" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="G25">
         <v>3</v>
@@ -1992,20 +2667,20 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="B26" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="C26" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D26">
         <v>1140</v>
       </c>
       <c r="E26" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="G26">
         <v>4</v>
@@ -2013,20 +2688,20 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="B27" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="C27" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D27">
         <v>900</v>
       </c>
       <c r="E27" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="G27">
         <v>5</v>
@@ -2034,20 +2709,20 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="B28" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="C28" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D28">
         <v>675</v>
       </c>
       <c r="E28" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="G28">
         <v>6</v>
@@ -2055,20 +2730,20 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="B29" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="C29" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D29">
         <v>15</v>
       </c>
       <c r="E29" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -2076,20 +2751,20 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="B30" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="C30" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D30">
         <v>40</v>
       </c>
       <c r="E30" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="G30">
         <v>1</v>
@@ -2097,20 +2772,20 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="B31" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="C31" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D31">
         <v>45</v>
       </c>
       <c r="E31" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="G31">
         <v>2</v>
@@ -2118,20 +2793,20 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="B32" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="C32" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D32">
         <v>130</v>
       </c>
       <c r="E32" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="G32">
         <v>3</v>
@@ -2139,20 +2814,20 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="B33" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="C33" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D33">
         <v>90</v>
       </c>
       <c r="E33" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="G33">
         <v>4</v>
@@ -2160,20 +2835,20 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="B34" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="C34" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D34">
         <v>120</v>
       </c>
       <c r="E34" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="G34">
         <v>5</v>
@@ -2181,20 +2856,20 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="B35" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="C35" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D35">
         <v>50</v>
       </c>
       <c r="E35" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="G35">
         <v>6</v>
@@ -2202,20 +2877,20 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="B36" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="C36" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D36">
         <v>25</v>
       </c>
       <c r="E36" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="G36">
         <v>7</v>
@@ -2223,20 +2898,20 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="B37" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="C37" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D37">
         <v>40</v>
       </c>
       <c r="E37" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="G37">
         <v>8</v>
@@ -2244,20 +2919,20 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="B38" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="C38" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D38">
         <v>50</v>
       </c>
       <c r="E38" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="G38">
         <v>9</v>
@@ -2265,20 +2940,20 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="B39" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="C39" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D39">
         <v>40</v>
       </c>
       <c r="E39" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="G39">
         <v>10</v>
@@ -2286,20 +2961,20 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="B40" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="C40" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D40">
         <v>80</v>
       </c>
       <c r="E40" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="G40">
         <v>11</v>
@@ -2307,20 +2982,20 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="B41" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="C41" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D41">
         <v>40</v>
       </c>
       <c r="E41" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="G41">
         <v>12</v>
@@ -2328,20 +3003,20 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="B42" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="C42" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D42">
         <v>270</v>
       </c>
       <c r="E42" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="G42">
         <v>13</v>
@@ -2349,20 +3024,20 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="B43" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="C43" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D43">
         <v>210</v>
       </c>
       <c r="E43" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="G43">
         <v>14</v>
@@ -2370,20 +3045,20 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="B44" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="C44" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D44">
         <v>170</v>
       </c>
       <c r="E44" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="G44">
         <v>15</v>
@@ -2391,20 +3066,20 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="B45" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="C45" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D45">
         <v>40</v>
       </c>
       <c r="E45" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="G45">
         <v>16</v>
@@ -2412,20 +3087,20 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="B46" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="C46" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D46">
         <v>35</v>
       </c>
       <c r="E46" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="G46">
         <v>17</v>
@@ -2433,20 +3108,20 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="B47" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="C47" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D47">
         <v>40</v>
       </c>
       <c r="E47" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="G47">
         <v>18</v>
@@ -2454,20 +3129,20 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="B48" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="C48" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D48">
         <v>110</v>
       </c>
       <c r="E48" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="G48">
         <v>19</v>
@@ -2475,20 +3150,20 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="B49" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="C49" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D49">
         <v>70</v>
       </c>
       <c r="E49" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="G49">
         <v>20</v>
@@ -2496,20 +3171,20 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="B50" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="C50" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D50">
         <v>370</v>
       </c>
       <c r="E50" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="G50">
         <v>21</v>
@@ -2517,20 +3192,20 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B51" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="C51" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D51">
         <v>30</v>
       </c>
       <c r="E51" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="G51">
         <v>22</v>
@@ -2538,20 +3213,20 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="B52" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="C52" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D52">
         <v>120</v>
       </c>
       <c r="E52" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="G52">
         <v>23</v>
@@ -2559,20 +3234,20 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="B53" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="C53" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D53">
         <v>130</v>
       </c>
       <c r="E53" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="G53">
         <v>24</v>
@@ -2580,20 +3255,20 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="B54" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="C54" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D54">
         <v>120</v>
       </c>
       <c r="E54" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="G54">
         <v>25</v>
@@ -2601,23 +3276,23 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="B55" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="C55" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D55">
         <v>480</v>
       </c>
       <c r="E55" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="F55" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="G55">
         <v>1</v>
@@ -2625,23 +3300,23 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="B56" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="C56" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D56">
         <v>960</v>
       </c>
       <c r="E56" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="F56" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="G56">
         <v>2</v>
@@ -2649,23 +3324,23 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="B57" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="C57" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D57">
         <v>960</v>
       </c>
       <c r="E57" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="F57" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="G57">
         <v>3</v>
@@ -2673,23 +3348,23 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="B58" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="C58" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D58">
         <v>1920</v>
       </c>
       <c r="E58" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="F58" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="G58">
         <v>4</v>
@@ -2697,23 +3372,23 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="B59" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
       <c r="C59" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D59">
         <v>1440</v>
       </c>
       <c r="E59" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="F59" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="G59">
         <v>5</v>
@@ -2730,12 +3405,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4884ACB8-CF81-4DD8-BC47-C124E0924889}">
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="G27" sqref="A2:G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2751,43 +3426,43 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="E1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="F1" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="G1" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="B2" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="C2" s="5">
         <f t="shared" ref="C2:C27" ca="1" si="0">NOW()</f>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D2">
         <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -2795,20 +3470,20 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="C3" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D3">
         <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -2816,20 +3491,20 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="B4" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="C4" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D4">
         <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="G4">
         <v>2</v>
@@ -2837,20 +3512,20 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="B5" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="C5" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D5">
         <v>120</v>
       </c>
       <c r="F5" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="G5">
         <v>3</v>
@@ -2858,20 +3533,20 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="B6" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="C6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D6">
         <v>60</v>
       </c>
       <c r="F6" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="G6">
         <v>4</v>
@@ -2879,20 +3554,20 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="B7" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="C7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D7">
         <v>5</v>
       </c>
       <c r="F7" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="G7">
         <v>5</v>
@@ -2900,20 +3575,20 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="B8" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="C8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D8">
         <v>25</v>
       </c>
       <c r="F8" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="G8">
         <v>6</v>
@@ -2921,20 +3596,20 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="B9" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="C9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D9">
         <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="G9">
         <v>7</v>
@@ -2942,20 +3617,20 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="B10" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D10">
         <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="G10">
         <v>8</v>
@@ -2963,20 +3638,20 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
       <c r="B11" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="C11" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D11">
         <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="G11">
         <v>9</v>
@@ -2984,20 +3659,20 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="B12" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="C12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D12">
         <v>25</v>
       </c>
       <c r="F12" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="G12">
         <v>10</v>
@@ -3005,20 +3680,20 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="B13" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="C13" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D13">
         <v>40</v>
       </c>
       <c r="F13" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="G13">
         <v>11</v>
@@ -3026,20 +3701,20 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="B14" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="C14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D14">
         <v>25</v>
       </c>
       <c r="F14" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="G14">
         <v>12</v>
@@ -3047,20 +3722,20 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="B15" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C15" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D15">
         <v>90</v>
       </c>
       <c r="F15" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="G15">
         <v>13</v>
@@ -3068,20 +3743,20 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B16" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="C16" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D16">
         <v>90</v>
       </c>
       <c r="F16" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="G16">
         <v>14</v>
@@ -3089,20 +3764,20 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
       <c r="B17" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="C17" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D17">
         <v>5</v>
       </c>
       <c r="F17" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="G17">
         <v>15</v>
@@ -3110,20 +3785,20 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="B18" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="C18" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D18">
         <v>5</v>
       </c>
       <c r="F18" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="G18">
         <v>16</v>
@@ -3131,20 +3806,20 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
       <c r="B19" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="C19" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D19">
         <v>90</v>
       </c>
       <c r="F19" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="G19">
         <v>17</v>
@@ -3152,20 +3827,20 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="B20" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C20" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D20">
         <v>25</v>
       </c>
       <c r="F20" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="G20">
         <v>18</v>
@@ -3173,20 +3848,20 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
       <c r="B21" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="C21" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D21">
         <v>120</v>
       </c>
       <c r="F21" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="G21">
         <v>19</v>
@@ -3194,20 +3869,20 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
       <c r="B22" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="C22" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D22">
         <v>50</v>
       </c>
       <c r="F22" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="G22">
         <v>20</v>
@@ -3215,20 +3890,20 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
       <c r="B23" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="C23" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D23">
         <v>180</v>
       </c>
       <c r="F23" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="G23">
         <v>21</v>
@@ -3236,20 +3911,20 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="B24" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="C24" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D24">
         <v>25</v>
       </c>
       <c r="F24" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="G24">
         <v>22</v>
@@ -3257,20 +3932,20 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="B25" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="C25" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D25">
         <v>5</v>
       </c>
       <c r="F25" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="G25">
         <v>23</v>
@@ -3278,20 +3953,20 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="B26" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="C26" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D26">
         <v>5</v>
       </c>
       <c r="F26" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="G26">
         <v>24</v>
@@ -3299,20 +3974,20 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="B27" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="C27" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D27">
         <v>5</v>
       </c>
       <c r="F27" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="G27">
         <v>25</v>
@@ -3351,12 +4026,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C368744-B552-4427-9047-A14205368F29}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3377,28 +4052,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E1" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="F1" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="G1" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="H1" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -3412,32 +4087,32 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+      <selection activeCell="A2" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="B2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="B4" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -3450,32 +4125,32 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="A2" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="B4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -3484,11 +4159,290 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD7B66B1-6BC6-4C30-9443-0722E61BBB20}">
+  <dimension ref="A1:P12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C1" t="s">
+        <v>302</v>
+      </c>
+      <c r="D1" t="s">
+        <v>303</v>
+      </c>
+      <c r="E1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F1" t="s">
+        <v>305</v>
+      </c>
+      <c r="G1" t="s">
+        <v>306</v>
+      </c>
+      <c r="H1" t="s">
+        <v>307</v>
+      </c>
+      <c r="I1" t="s">
+        <v>308</v>
+      </c>
+      <c r="J1" t="s">
+        <v>296</v>
+      </c>
+      <c r="K1" t="s">
+        <v>309</v>
+      </c>
+      <c r="L1" t="s">
+        <v>310</v>
+      </c>
+      <c r="M1" t="s">
+        <v>311</v>
+      </c>
+      <c r="N1" t="s">
+        <v>312</v>
+      </c>
+      <c r="O1" t="s">
+        <v>313</v>
+      </c>
+      <c r="P1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B2" s="5">
+        <v>45751.562223726854</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="I2" t="s">
+        <v>320</v>
+      </c>
+      <c r="J2" t="s">
+        <v>323</v>
+      </c>
+      <c r="L2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
+        <v>327</v>
+      </c>
+      <c r="B3" s="5">
+        <v>45752.562223726854</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="I3" t="s">
+        <v>321</v>
+      </c>
+      <c r="J3" t="s">
+        <v>324</v>
+      </c>
+      <c r="L3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" t="s">
+        <v>328</v>
+      </c>
+      <c r="B4" s="5">
+        <v>45753.562223726854</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="I4" t="s">
+        <v>322</v>
+      </c>
+      <c r="J4" t="s">
+        <v>332</v>
+      </c>
+      <c r="L4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="H5" s="7"/>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="F10" s="1"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="F11" s="1"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="F12" s="1"/>
+      <c r="H12" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{542E9486-D6E1-4A7E-A8BE-9D54E56CA329}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="37.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>327</v>
+      </c>
+      <c r="B3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>328</v>
+      </c>
+      <c r="B4" t="s">
+        <v>288</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D42C8E0E-79CC-41C9-948F-342BD1A37C0C}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3503,75 +4457,66 @@
     <col min="8" max="8" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>306</v>
+        <v>335</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>336</v>
+      </c>
+      <c r="E1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>327</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>328</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>333</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>333</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" t="s">
-        <v>307</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -3579,112 +4524,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD7B66B1-6BC6-4C30-9443-0722E61BBB20}">
-  <dimension ref="A1:H5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>302</v>
-      </c>
-      <c r="C1" t="s">
-        <v>303</v>
-      </c>
-      <c r="D1" t="s">
-        <v>304</v>
-      </c>
-      <c r="E1" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>308</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="5">
-        <v>45751.562223726854</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>309</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="5">
-        <v>45751.562223726854</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>307</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="5">
-        <v>45751.562223726854</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="H4" s="8"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="H5" s="7"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{04545774-7793-45A9-8AF5-0E41294C9250}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{25181597-4BC6-468B-8E5D-9759FFD45830}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{E0FF25A3-DEBD-41F2-9BFB-8533EB890262}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978806DB-8FE4-474B-99FD-427CEAAF2910}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -3694,49 +4534,49 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="F1" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="C2" s="6">
         <f ca="1">NOW()</f>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="2"/>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -3745,12 +4585,38 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E6B77D2-2052-4B42-B49C-F3748ED79E13}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B88C5E0D-19FC-476E-B097-DA7E154320DE}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3767,40 +4633,40 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="F1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="C2" s="6">
         <f ca="1">NOW()</f>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -3808,20 +4674,20 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="C3" s="6">
         <f ca="1">NOW()</f>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="E3" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -3829,20 +4695,20 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="C4" s="6">
         <f ca="1">NOW()</f>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -3850,20 +4716,20 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="C5" s="6">
         <f ca="1">NOW()</f>
-        <v>45754.005903703706</v>
+        <v>45755.53341689815</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="E5" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -3873,542 +4739,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7122162C-AD73-4663-9975-8D7C83047E49}">
-  <dimension ref="A1:F29"/>
-  <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="84.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="122.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="6">
-        <f t="shared" ref="C2:C12" ca="1" si="0">NOW()</f>
-        <v>45754.005903703706</v>
-      </c>
-      <c r="D2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
-      </c>
-      <c r="D3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C4" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
-      </c>
-      <c r="D4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
-      </c>
-      <c r="D5" t="s">
-        <v>86</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>106</v>
-      </c>
-      <c r="B6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C6" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
-      </c>
-      <c r="D6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>107</v>
-      </c>
-      <c r="B7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
-      </c>
-      <c r="D7" t="s">
-        <v>88</v>
-      </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>108</v>
-      </c>
-      <c r="B8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
-      </c>
-      <c r="D8" t="s">
-        <v>88</v>
-      </c>
-      <c r="E8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>109</v>
-      </c>
-      <c r="B9" t="s">
-        <v>74</v>
-      </c>
-      <c r="C9" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>110</v>
-      </c>
-      <c r="B10" t="s">
-        <v>93</v>
-      </c>
-      <c r="C10" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>111</v>
-      </c>
-      <c r="B11" t="s">
-        <v>101</v>
-      </c>
-      <c r="C11" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
-      </c>
-      <c r="D11" t="s">
-        <v>91</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>112</v>
-      </c>
-      <c r="B12" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2">
-      <c r="B19" s="4"/>
-    </row>
-    <row r="20" spans="2:2">
-      <c r="B20" s="4"/>
-    </row>
-    <row r="21" spans="2:2">
-      <c r="B21" s="4"/>
-    </row>
-    <row r="22" spans="2:2">
-      <c r="B22" s="4"/>
-    </row>
-    <row r="23" spans="2:2">
-      <c r="B23" s="4"/>
-    </row>
-    <row r="24" spans="2:2">
-      <c r="B24" s="4"/>
-    </row>
-    <row r="25" spans="2:2">
-      <c r="B25" s="4"/>
-    </row>
-    <row r="26" spans="2:2">
-      <c r="B26" s="4"/>
-    </row>
-    <row r="27" spans="2:2">
-      <c r="B27" s="4"/>
-    </row>
-    <row r="28" spans="2:2">
-      <c r="B28" s="4"/>
-    </row>
-    <row r="29" spans="2:2">
-      <c r="B29" s="4"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D10" r:id="rId1" xr:uid="{223B1678-144B-4D76-9D65-D27BD252BBF2}"/>
-    <hyperlink ref="D12" r:id="rId2" xr:uid="{C6D3A5D0-19B9-49D5-A5EE-452D74ABD85D}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5370AC90-9927-445C-B04F-4A41A0706261}">
-  <dimension ref="A1:O13"/>
-  <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="69.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="39.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="33" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="62.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D2" s="6">
-        <f ca="1">NOW()</f>
-        <v>45754.005903703706</v>
-      </c>
-      <c r="F2">
-        <v>480</v>
-      </c>
-      <c r="O2" s="2"/>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D3" s="6">
-        <f t="shared" ref="D3:D13" ca="1" si="0">NOW()</f>
-        <v>45754.005903703706</v>
-      </c>
-      <c r="F3">
-        <v>960</v>
-      </c>
-      <c r="O3" s="2"/>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="A4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D4" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
-      </c>
-      <c r="F4">
-        <v>480</v>
-      </c>
-      <c r="O4" s="2"/>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D5" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
-      </c>
-      <c r="F5">
-        <v>1440</v>
-      </c>
-      <c r="O5" s="2"/>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D6" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" t="s">
-        <v>120</v>
-      </c>
-      <c r="B7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C7" t="s">
-        <v>107</v>
-      </c>
-      <c r="D7" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" t="s">
-        <v>121</v>
-      </c>
-      <c r="B8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C8" t="s">
-        <v>108</v>
-      </c>
-      <c r="D8" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" t="s">
-        <v>122</v>
-      </c>
-      <c r="B9" t="s">
-        <v>100</v>
-      </c>
-      <c r="C9" t="s">
-        <v>109</v>
-      </c>
-      <c r="D9" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" t="s">
-        <v>123</v>
-      </c>
-      <c r="B10" t="s">
-        <v>97</v>
-      </c>
-      <c r="C10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D10" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
-      </c>
-      <c r="E10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" t="s">
-        <v>124</v>
-      </c>
-      <c r="B11" t="s">
-        <v>98</v>
-      </c>
-      <c r="C11" t="s">
-        <v>111</v>
-      </c>
-      <c r="D11" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
-      </c>
-      <c r="E11" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="A12" t="s">
-        <v>125</v>
-      </c>
-      <c r="B12" t="s">
-        <v>99</v>
-      </c>
-      <c r="C12" t="s">
-        <v>112</v>
-      </c>
-      <c r="D12" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
-      </c>
-      <c r="E12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="A13" t="s">
-        <v>126</v>
-      </c>
-      <c r="B13" t="s">
-        <v>98</v>
-      </c>
-      <c r="C13" t="s">
-        <v>106</v>
-      </c>
-      <c r="D13" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>45754.005903703706</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
fix: commit no saved data
</commit_message>
<xml_diff>
--- a/database/data_for_import/data_for_import.xlsx
+++ b/database/data_for_import/data_for_import.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Progects\study_1c\database\data_for_import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Progect\pp+diplom\study_1c\database\data_for_import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB11441F-061D-48B2-9F4F-AA08C34C10A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D70543-F777-4715-85EC-EB43CA11BE6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="775" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" tabRatio="775" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="roles" sheetId="1" r:id="rId1"/>
@@ -1574,18 +1574,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7122162C-AD73-4663-9975-8D7C83047E49}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F12"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="84.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="122.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="95.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="133" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
@@ -1629,7 +1629,7 @@
       </c>
       <c r="C2" s="6">
         <f t="shared" ref="C2:C12" ca="1" si="0">NOW()</f>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D2" t="s">
         <v>67</v>
@@ -1647,7 +1647,7 @@
       </c>
       <c r="C3" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D3" t="s">
         <v>68</v>
@@ -1665,7 +1665,7 @@
       </c>
       <c r="C4" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D4" t="s">
         <v>70</v>
@@ -1683,7 +1683,7 @@
       </c>
       <c r="C5" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D5" t="s">
         <v>72</v>
@@ -1701,7 +1701,7 @@
       </c>
       <c r="C6" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D6" t="s">
         <v>74</v>
@@ -1719,7 +1719,7 @@
       </c>
       <c r="C7" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D7" t="s">
         <v>74</v>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="C8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D8" t="s">
         <v>74</v>
@@ -1755,7 +1755,7 @@
       </c>
       <c r="C9" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -1770,7 +1770,7 @@
       </c>
       <c r="C10" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>76</v>
@@ -1788,7 +1788,7 @@
       </c>
       <c r="C11" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D11" t="s">
         <v>77</v>
@@ -1806,7 +1806,7 @@
       </c>
       <c r="C12" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>78</v>
@@ -1862,17 +1862,16 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F13"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="69.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="76.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="39.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="33" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="62.140625" bestFit="1" customWidth="1"/>
@@ -1910,7 +1909,7 @@
       </c>
       <c r="D2" s="6">
         <f ca="1">NOW()</f>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="F2">
         <v>480</v>
@@ -1929,7 +1928,7 @@
       </c>
       <c r="D3" s="6">
         <f t="shared" ref="D3:D13" ca="1" si="0">NOW()</f>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="F3">
         <v>960</v>
@@ -1948,7 +1947,7 @@
       </c>
       <c r="D4" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="F4">
         <v>480</v>
@@ -1967,7 +1966,7 @@
       </c>
       <c r="D5" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="F5">
         <v>1440</v>
@@ -1986,7 +1985,7 @@
       </c>
       <c r="D6" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -2001,7 +2000,7 @@
       </c>
       <c r="D7" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -2016,7 +2015,7 @@
       </c>
       <c r="D8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -2031,7 +2030,7 @@
       </c>
       <c r="D9" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -2046,7 +2045,7 @@
       </c>
       <c r="D10" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="E10" t="s">
         <v>81</v>
@@ -2064,7 +2063,7 @@
       </c>
       <c r="D11" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="E11" t="s">
         <v>99</v>
@@ -2082,7 +2081,7 @@
       </c>
       <c r="D12" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="E12" t="s">
         <v>100</v>
@@ -2100,7 +2099,7 @@
       </c>
       <c r="D13" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
     </row>
   </sheetData>
@@ -2112,20 +2111,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666A1DBF-4A90-426C-A8FE-B6C9014C9F32}">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H59"/>
+    <sheetView topLeftCell="B44" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40.85546875" customWidth="1"/>
-    <col min="2" max="2" width="127" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="139.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="33" bestFit="1" customWidth="1"/>
@@ -2170,7 +2169,7 @@
       </c>
       <c r="C2" s="5">
         <f ca="1">NOW()</f>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D2">
         <v>50</v>
@@ -2191,7 +2190,7 @@
       </c>
       <c r="C3" s="5">
         <f t="shared" ref="C3:C59" ca="1" si="0">NOW()</f>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D3">
         <v>50</v>
@@ -2212,7 +2211,7 @@
       </c>
       <c r="C4" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D4">
         <v>50</v>
@@ -2233,7 +2232,7 @@
       </c>
       <c r="C5" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D5">
         <v>50</v>
@@ -2254,7 +2253,7 @@
       </c>
       <c r="C6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D6">
         <v>50</v>
@@ -2275,7 +2274,7 @@
       </c>
       <c r="C7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D7">
         <v>50</v>
@@ -2296,7 +2295,7 @@
       </c>
       <c r="C8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D8">
         <v>60</v>
@@ -2317,7 +2316,7 @@
       </c>
       <c r="C9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D9">
         <v>60</v>
@@ -2338,7 +2337,7 @@
       </c>
       <c r="C10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D10">
         <v>60</v>
@@ -2359,7 +2358,7 @@
       </c>
       <c r="C11" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D11">
         <v>60</v>
@@ -2380,7 +2379,7 @@
       </c>
       <c r="C12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D12">
         <v>60</v>
@@ -2401,7 +2400,7 @@
       </c>
       <c r="C13" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D13">
         <v>60</v>
@@ -2422,7 +2421,7 @@
       </c>
       <c r="C14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D14">
         <v>60</v>
@@ -2443,7 +2442,7 @@
       </c>
       <c r="C15" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D15">
         <v>60</v>
@@ -2464,7 +2463,7 @@
       </c>
       <c r="C16" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D16">
         <v>60</v>
@@ -2485,7 +2484,7 @@
       </c>
       <c r="C17" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D17">
         <v>60</v>
@@ -2506,7 +2505,7 @@
       </c>
       <c r="C18" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D18">
         <v>60</v>
@@ -2527,7 +2526,7 @@
       </c>
       <c r="C19" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D19">
         <v>60</v>
@@ -2548,7 +2547,7 @@
       </c>
       <c r="C20" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D20">
         <v>60</v>
@@ -2569,7 +2568,7 @@
       </c>
       <c r="C21" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D21">
         <v>60</v>
@@ -2590,7 +2589,7 @@
       </c>
       <c r="C22" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D22">
         <v>60</v>
@@ -2611,7 +2610,7 @@
       </c>
       <c r="C23" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D23">
         <v>1035</v>
@@ -2632,7 +2631,7 @@
       </c>
       <c r="C24" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D24">
         <v>1320</v>
@@ -2653,7 +2652,7 @@
       </c>
       <c r="C25" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D25">
         <v>1200</v>
@@ -2674,7 +2673,7 @@
       </c>
       <c r="C26" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D26">
         <v>1140</v>
@@ -2695,7 +2694,7 @@
       </c>
       <c r="C27" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D27">
         <v>900</v>
@@ -2716,7 +2715,7 @@
       </c>
       <c r="C28" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D28">
         <v>675</v>
@@ -2737,7 +2736,7 @@
       </c>
       <c r="C29" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D29">
         <v>15</v>
@@ -2758,7 +2757,7 @@
       </c>
       <c r="C30" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D30">
         <v>40</v>
@@ -2779,7 +2778,7 @@
       </c>
       <c r="C31" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D31">
         <v>45</v>
@@ -2800,7 +2799,7 @@
       </c>
       <c r="C32" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D32">
         <v>130</v>
@@ -2821,7 +2820,7 @@
       </c>
       <c r="C33" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D33">
         <v>90</v>
@@ -2842,7 +2841,7 @@
       </c>
       <c r="C34" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D34">
         <v>120</v>
@@ -2863,7 +2862,7 @@
       </c>
       <c r="C35" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D35">
         <v>50</v>
@@ -2884,7 +2883,7 @@
       </c>
       <c r="C36" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D36">
         <v>25</v>
@@ -2905,7 +2904,7 @@
       </c>
       <c r="C37" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D37">
         <v>40</v>
@@ -2926,7 +2925,7 @@
       </c>
       <c r="C38" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D38">
         <v>50</v>
@@ -2947,7 +2946,7 @@
       </c>
       <c r="C39" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D39">
         <v>40</v>
@@ -2968,7 +2967,7 @@
       </c>
       <c r="C40" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D40">
         <v>80</v>
@@ -2989,7 +2988,7 @@
       </c>
       <c r="C41" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D41">
         <v>40</v>
@@ -3010,7 +3009,7 @@
       </c>
       <c r="C42" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D42">
         <v>270</v>
@@ -3031,7 +3030,7 @@
       </c>
       <c r="C43" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D43">
         <v>210</v>
@@ -3052,7 +3051,7 @@
       </c>
       <c r="C44" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D44">
         <v>170</v>
@@ -3073,7 +3072,7 @@
       </c>
       <c r="C45" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D45">
         <v>40</v>
@@ -3094,7 +3093,7 @@
       </c>
       <c r="C46" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D46">
         <v>35</v>
@@ -3115,7 +3114,7 @@
       </c>
       <c r="C47" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D47">
         <v>40</v>
@@ -3136,7 +3135,7 @@
       </c>
       <c r="C48" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D48">
         <v>110</v>
@@ -3157,7 +3156,7 @@
       </c>
       <c r="C49" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D49">
         <v>70</v>
@@ -3178,7 +3177,7 @@
       </c>
       <c r="C50" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D50">
         <v>370</v>
@@ -3199,7 +3198,7 @@
       </c>
       <c r="C51" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D51">
         <v>30</v>
@@ -3220,7 +3219,7 @@
       </c>
       <c r="C52" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D52">
         <v>120</v>
@@ -3241,7 +3240,7 @@
       </c>
       <c r="C53" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D53">
         <v>130</v>
@@ -3262,7 +3261,7 @@
       </c>
       <c r="C54" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D54">
         <v>120</v>
@@ -3283,7 +3282,7 @@
       </c>
       <c r="C55" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D55">
         <v>480</v>
@@ -3307,7 +3306,7 @@
       </c>
       <c r="C56" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D56">
         <v>960</v>
@@ -3331,7 +3330,7 @@
       </c>
       <c r="C57" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D57">
         <v>960</v>
@@ -3355,7 +3354,7 @@
       </c>
       <c r="C58" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D58">
         <v>1920</v>
@@ -3379,7 +3378,7 @@
       </c>
       <c r="C59" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D59">
         <v>1440</v>
@@ -3410,7 +3409,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G27" sqref="A2:G27"/>
+      <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3456,7 +3455,7 @@
       </c>
       <c r="C2" s="5">
         <f t="shared" ref="C2:C27" ca="1" si="0">NOW()</f>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D2">
         <v>5</v>
@@ -3477,7 +3476,7 @@
       </c>
       <c r="C3" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D3">
         <v>20</v>
@@ -3498,7 +3497,7 @@
       </c>
       <c r="C4" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D4">
         <v>25</v>
@@ -3519,7 +3518,7 @@
       </c>
       <c r="C5" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D5">
         <v>120</v>
@@ -3540,7 +3539,7 @@
       </c>
       <c r="C6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D6">
         <v>60</v>
@@ -3561,7 +3560,7 @@
       </c>
       <c r="C7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -3582,7 +3581,7 @@
       </c>
       <c r="C8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D8">
         <v>25</v>
@@ -3603,7 +3602,7 @@
       </c>
       <c r="C9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D9">
         <v>15</v>
@@ -3624,7 +3623,7 @@
       </c>
       <c r="C10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D10">
         <v>25</v>
@@ -3645,7 +3644,7 @@
       </c>
       <c r="C11" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D11">
         <v>25</v>
@@ -3666,7 +3665,7 @@
       </c>
       <c r="C12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D12">
         <v>25</v>
@@ -3687,7 +3686,7 @@
       </c>
       <c r="C13" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D13">
         <v>40</v>
@@ -3708,7 +3707,7 @@
       </c>
       <c r="C14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D14">
         <v>25</v>
@@ -3729,7 +3728,7 @@
       </c>
       <c r="C15" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D15">
         <v>90</v>
@@ -3750,7 +3749,7 @@
       </c>
       <c r="C16" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D16">
         <v>90</v>
@@ -3771,7 +3770,7 @@
       </c>
       <c r="C17" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D17">
         <v>5</v>
@@ -3792,7 +3791,7 @@
       </c>
       <c r="C18" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D18">
         <v>5</v>
@@ -3813,7 +3812,7 @@
       </c>
       <c r="C19" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D19">
         <v>90</v>
@@ -3834,7 +3833,7 @@
       </c>
       <c r="C20" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D20">
         <v>25</v>
@@ -3855,7 +3854,7 @@
       </c>
       <c r="C21" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D21">
         <v>120</v>
@@ -3876,7 +3875,7 @@
       </c>
       <c r="C22" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D22">
         <v>50</v>
@@ -3897,7 +3896,7 @@
       </c>
       <c r="C23" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D23">
         <v>180</v>
@@ -3918,7 +3917,7 @@
       </c>
       <c r="C24" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D24">
         <v>25</v>
@@ -3939,7 +3938,7 @@
       </c>
       <c r="C25" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D25">
         <v>5</v>
@@ -3960,7 +3959,7 @@
       </c>
       <c r="C26" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D26">
         <v>5</v>
@@ -3981,7 +3980,7 @@
       </c>
       <c r="C27" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D27">
         <v>5</v>
@@ -4030,8 +4029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C368744-B552-4427-9047-A14205368F29}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4392,7 +4391,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4529,7 +4528,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F2"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4571,7 +4570,7 @@
       </c>
       <c r="C2" s="6">
         <f ca="1">NOW()</f>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="2"/>
@@ -4616,17 +4615,17 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F5"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="18" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -4660,7 +4659,7 @@
       </c>
       <c r="C2" s="6">
         <f ca="1">NOW()</f>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>53</v>
@@ -4681,7 +4680,7 @@
       </c>
       <c r="C3" s="6">
         <f ca="1">NOW()</f>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>53</v>
@@ -4702,7 +4701,7 @@
       </c>
       <c r="C4" s="6">
         <f ca="1">NOW()</f>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>53</v>
@@ -4723,7 +4722,7 @@
       </c>
       <c r="C5" s="6">
         <f ca="1">NOW()</f>
-        <v>45755.53341689815</v>
+        <v>45761.034055324075</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>53</v>

</xml_diff>